<commit_message>
Updated README.md with proper minimal example
Signed-off-by: JasonMendoza2008 <lhotteromain@gmail.com>
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CEFBD3-CE94-489A-B0A9-3956EC04F4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEB2C0F-02C1-4750-8966-6C83C2104ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19298" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="False Negatives" sheetId="8" r:id="rId1"/>
+    <sheet name="My Sheet" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'False Negatives'!$A$1:$W$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'My Sheet'!$A$1:$W$1</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>

</xml_diff>

<commit_message>
Upgrade towards supporting DQA1, DRB345, DPB1 and DPA1
Not all tests pass
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112FDBD4-523C-485B-A14F-A72BA8A5B787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BFB18B-8588-41AE-96EE-B0F2C1E30CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="2268" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="My Sheet" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'My Sheet'!$A$1:$W$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'My Sheet'!$A$1:$AI$1</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="72">
   <si>
     <t>A*01:01</t>
   </si>
@@ -188,6 +188,66 @@
   </si>
   <si>
     <t>C2_R</t>
+  </si>
+  <si>
+    <t>DRB3451_D</t>
+  </si>
+  <si>
+    <t>DRB3452_D</t>
+  </si>
+  <si>
+    <t>DRB345*</t>
+  </si>
+  <si>
+    <t>DQA12_D</t>
+  </si>
+  <si>
+    <t>DQA11_D</t>
+  </si>
+  <si>
+    <t>DQA1*</t>
+  </si>
+  <si>
+    <t>DRB3451_R</t>
+  </si>
+  <si>
+    <t>DRB3452_R</t>
+  </si>
+  <si>
+    <t>DQA11_R</t>
+  </si>
+  <si>
+    <t>DQA12_R</t>
+  </si>
+  <si>
+    <t>DPA11_D</t>
+  </si>
+  <si>
+    <t>DPA12_D</t>
+  </si>
+  <si>
+    <t>DPB11_D</t>
+  </si>
+  <si>
+    <t>DPB12_D</t>
+  </si>
+  <si>
+    <t>DPA1*</t>
+  </si>
+  <si>
+    <t>DPB1*</t>
+  </si>
+  <si>
+    <t>DPA11_R</t>
+  </si>
+  <si>
+    <t>DPA12_R</t>
+  </si>
+  <si>
+    <t>DPB11_R</t>
+  </si>
+  <si>
+    <t>DPB12_R</t>
   </si>
 </sst>
 </file>
@@ -558,16 +618,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F970583-F056-4017-A8C5-0EF95FF28D3C}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:AM4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="12.81640625" style="2"/>
+    <col min="1" max="18" width="12.81640625" style="2"/>
+    <col min="19" max="19" width="12.81640625" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="12.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -596,43 +658,91 @@
         <v>33</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="AJ1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -661,43 +771,91 @@
         <v>7</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="AD2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="AJ2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -726,43 +884,91 @@
         <v>17</v>
       </c>
       <c r="K3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="V3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Y3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="Z3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="AA3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="AB3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="AC3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="AD3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="AI3" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="AJ3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM3" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -791,40 +997,88 @@
         <v>26</v>
       </c>
       <c r="K4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="V4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="X4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="Z4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="AA4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="AB4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="AC4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="4" t="s">
+      <c r="AD4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="AI4" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="AJ4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM4" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>